<commit_message>
Updated Project Plan and Task Allocation
</commit_message>
<xml_diff>
--- a/docs/Deliverable2-Task Allocation.xlsx
+++ b/docs/Deliverable2-Task Allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\YanData\Langara\T4 - 2022 Fall\CPSC-2350-M01-Software Practice\Group Project\project-workspace\allin1store.github.io\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8723E7A8-6198-466C-84B9-5C2495C17A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C4A4C6-6292-49C0-9797-54A40A6BA6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12652" xr2:uid="{D6CD711B-E1C6-43BA-9FE4-882CDD526EEE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>T1</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Sprint 3</t>
   </si>
   <si>
-    <t>Sprint 4</t>
-  </si>
-  <si>
     <t>Website Templates</t>
   </si>
   <si>
@@ -111,12 +108,6 @@
   </si>
   <si>
     <t>Estimated Days</t>
-  </si>
-  <si>
-    <t>Sprint 5</t>
-  </si>
-  <si>
-    <t>Sprint 6</t>
   </si>
 </sst>
 </file>
@@ -146,7 +137,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -231,6 +222,39 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color theme="8"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="8"/>
+      </top>
+      <bottom style="thick">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="8"/>
+      </top>
+      <bottom style="thick">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -238,9 +262,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thick">
-        <color theme="8"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -251,49 +273,38 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thick">
-        <color theme="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="8"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color theme="8"/>
-      </top>
-      <bottom style="thick">
-        <color theme="8"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="8"/>
+      </left>
+      <right style="thick">
+        <color theme="8"/>
+      </right>
       <top style="thick">
         <color theme="8"/>
       </top>
       <bottom style="thick">
         <color theme="8"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color theme="8"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -301,19 +312,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -321,10 +323,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -657,21 +673,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8301D496-5CBE-4DC1-8D4A-88AF0AF01654}">
-  <dimension ref="A2:O23"/>
+  <dimension ref="A2:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="1" max="1" width="11.0703125" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="19" width="5.640625" customWidth="1"/>
+    <col min="4" max="13" width="5.640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -679,21 +693,21 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -704,18 +718,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -726,7 +740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -737,50 +751,38 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:9">
       <c r="D12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:9">
       <c r="C14" s="6"/>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="11" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="11" t="s">
+      <c r="G14" s="9"/>
+      <c r="H14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="12"/>
-      <c r="L14" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="M14" s="12"/>
-      <c r="N14" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="O14" s="12"/>
-    </row>
-    <row r="15" spans="1:15" ht="14.6" thickBot="1">
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" ht="14.6" thickBot="1">
       <c r="C15" s="7" t="s">
         <v>2</v>
       </c>
@@ -788,49 +790,31 @@
         <v>1</v>
       </c>
       <c r="E15" s="14"/>
-      <c r="F15" s="11">
+      <c r="F15" s="8">
         <v>2</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="11">
+      <c r="G15" s="9"/>
+      <c r="H15" s="13">
         <v>3</v>
       </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="11">
-        <v>4</v>
-      </c>
-      <c r="K15" s="12"/>
-      <c r="L15" s="13">
-        <v>5</v>
-      </c>
-      <c r="M15" s="14"/>
-      <c r="N15" s="11">
-        <v>6</v>
-      </c>
-      <c r="O15" s="12"/>
-    </row>
-    <row r="16" spans="1:15" ht="15" thickTop="1" thickBot="1">
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickTop="1" thickBot="1">
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="M16" s="9"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-    </row>
-    <row r="17" spans="3:15" ht="15" thickTop="1" thickBot="1">
+    </row>
+    <row r="17" spans="3:9" ht="15" thickTop="1" thickBot="1">
       <c r="C17" s="2"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -838,35 +822,21 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-    </row>
-    <row r="18" spans="3:15" ht="15" thickTop="1" thickBot="1">
+    </row>
+    <row r="18" spans="3:9" ht="15" thickTop="1" thickBot="1">
       <c r="C18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="8" t="s">
+      <c r="D18" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="8" t="s">
+      <c r="E18" s="11"/>
+      <c r="H18" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-    </row>
-    <row r="19" spans="3:15" ht="15" thickTop="1" thickBot="1">
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="3:9" ht="15" thickTop="1" thickBot="1">
       <c r="C19" s="2"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -874,35 +844,21 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-    </row>
-    <row r="20" spans="3:15" ht="15" thickTop="1" thickBot="1">
+    </row>
+    <row r="20" spans="3:9" ht="15" thickTop="1" thickBot="1">
       <c r="C20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="9"/>
-      <c r="J20" s="8" t="s">
+      <c r="E20" s="11"/>
+      <c r="F20" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="9"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-    </row>
-    <row r="21" spans="3:15" ht="15" thickTop="1" thickBot="1">
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="3:9" ht="15" thickTop="1" thickBot="1">
       <c r="C21" s="2"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -910,14 +866,8 @@
       <c r="G21" s="5"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-    </row>
-    <row r="22" spans="3:15" ht="15" thickTop="1" thickBot="1">
+    </row>
+    <row r="22" spans="3:9" ht="15" thickTop="1" thickBot="1">
       <c r="C22" s="2" t="s">
         <v>6</v>
       </c>
@@ -925,15 +875,12 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="8" t="s">
+      <c r="H22" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M22" s="9"/>
-    </row>
-    <row r="23" spans="3:15" ht="14.6" thickTop="1">
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="3:9" ht="14.6" thickTop="1">
       <c r="C23" s="3"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -941,35 +888,21 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="12">
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="H22:I22"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D20:E20"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
     <mergeCell ref="H18:I18"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>